<commit_message>
Added remarks in xlsx.
</commit_message>
<xml_diff>
--- a/6/data.xlsx
+++ b/6/data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claus\CloudStation\Bsc 2020\2 semester\DSC\assignments\6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6E29C33E-E902-410C-891A-07F35A7C94FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB7C817-1D4E-471B-8FF5-2250C92B44BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>SampleDate</t>
   </si>
@@ -51,11 +62,20 @@
   <si>
     <t>t-test</t>
   </si>
+  <si>
+    <t>Vores t-test er ekstremt lille og viser faktisk at der er mere end 99% sandsynlighed for, at data ikke er tilfældige.</t>
+  </si>
+  <si>
+    <t>OBS: t-test er two-tailed og paired (fordi data hænger sammen med SampleDate)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qvPWQ-e03tQ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -890,11 +910,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L406"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +923,7 @@
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43887</v>
       </c>
@@ -968,7 +988,7 @@
         <v>6.340740740740741</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43888</v>
       </c>
@@ -1004,7 +1024,7 @@
         <v>10.127212793136914</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43889</v>
       </c>
@@ -1040,7 +1060,7 @@
         <v>102.56043895747598</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43891</v>
       </c>
@@ -1076,7 +1096,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43892</v>
       </c>
@@ -1096,11 +1116,11 @@
         <v>9</v>
       </c>
       <c r="I6">
-        <f>TTEST(B2:B406,C2:C406,2,2)</f>
-        <v>3.5305721888734969E-15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <f>TTEST(B2:B406,C2:C406,2,1)</f>
+        <v>4.7734185491325952E-33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43893</v>
       </c>
@@ -1116,8 +1136,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43894</v>
       </c>
@@ -1133,8 +1156,14 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43895</v>
       </c>
@@ -1151,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43896</v>
       </c>
@@ -1168,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43897</v>
       </c>
@@ -1185,7 +1214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43898</v>
       </c>
@@ -1202,7 +1231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43899</v>
       </c>
@@ -1219,7 +1248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43900</v>
       </c>
@@ -1236,7 +1265,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43901</v>
       </c>
@@ -1253,7 +1282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43902</v>
       </c>

</xml_diff>